<commit_message>
New updates related to summarization and updates to presentation materials in spreadsheet.
</commit_message>
<xml_diff>
--- a/Model Comparison Summary.xlsx
+++ b/Model Comparison Summary.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Learning\ML\NLP\Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CF3D8C3-8371-4441-A577-2AE749D877CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC1E55D-7DDE-4073-B001-3AF5ADC3B9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C0C7A1B3-45A7-49EE-AF3E-875ABE721FC4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{C0C7A1B3-45A7-49EE-AF3E-875ABE721FC4}"/>
   </bookViews>
   <sheets>
     <sheet name="LDA" sheetId="1" r:id="rId1"/>
-    <sheet name="BERTopic" sheetId="2" r:id="rId2"/>
-    <sheet name="Comparison Summary" sheetId="3" r:id="rId3"/>
+    <sheet name="MMR" sheetId="5" r:id="rId2"/>
+    <sheet name="BERTopic" sheetId="2" r:id="rId3"/>
+    <sheet name="Comparison Summary" sheetId="3" r:id="rId4"/>
+    <sheet name="Queries" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -116,6 +118,45 @@
   </si>
   <si>
     <t>Scalability on very large datasets</t>
+  </si>
+  <si>
+    <t>I am going through some tough times. I barely sleep and feel worthless. I tried to fix many things but nothig is helping. How can I get over feeling worthless?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I took a job away from home. I really need this job but being away from home makes me feel really depressed. Could you please help?</t>
+  </si>
+  <si>
+    <t>I am going through counseling for my depression. I feel very nervous and shaky when I go through the session. Is this normal?</t>
+  </si>
+  <si>
+    <t>I am feeling very depressed because of the winter weather. It makes me feel very sad.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I am a cancer survivor. I am also insomniac and have history of depression. Do I have too many issues to address in counseling?</t>
+  </si>
+  <si>
+    <t>I have lost connection with the world. Every one is so busy in their life. I want to drink every day and feel I have addiction issues. Could you please help?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I am in bad relationship. My boyfriend has been cheating on me. I feel like crying all the time.</t>
+  </si>
+  <si>
+    <t>I can not sleep and wake up at 2 'o clock in the morning. I eat a lot of sugar. Is that an issue?</t>
+  </si>
+  <si>
+    <t>Maximum Marginal Relevance (MMR)</t>
+  </si>
+  <si>
+    <t>Maximum Marginal Relevance (MMR) is a technique used in information retrieval and text summarization to balance two objectives:</t>
+  </si>
+  <si>
+    <t>1. Relevance: How relevant a candidate item (e.g., a document, sentence, or keyword) is to the query or topic of interest.</t>
+  </si>
+  <si>
+    <t>2. Diversity: How dissimilar the candidate item is from the items already selected, ensuring the final results are not redundant.</t>
+  </si>
+  <si>
+    <t>MMR is designed to select items that are not only relevant but also contribute new information to the result set.</t>
   </si>
 </sst>
 </file>
@@ -2957,6 +2998,55 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>274918</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>160421</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04AE20B0-06BD-B2F8-A394-36CC9A53746E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="2118360"/>
+          <a:ext cx="6904318" cy="4625741"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
       <xdr:row>4</xdr:row>
@@ -3321,8 +3411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29AD6B4C-C9AA-43DA-AFCB-EF99B513F570}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3467,11 +3557,52 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F371D4-51FB-4B02-9ADD-DBC2FFFBB06B}">
+  <dimension ref="B1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D28055-8EC3-4B00-9DEB-BD64C1F32F74}">
   <dimension ref="A6:B7"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3501,12 +3632,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F4B675-CB5A-46FC-B70D-11AB2E147F3D}">
   <dimension ref="A3:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3624,4 +3755,86 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91192709-FEC4-45CD-990C-D5E18F766D3A}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="132.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>